<commit_message>
update file checklist PSWeb
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/AREAS_PSWEB/20.15.00/accreditamento-checklist_AREAS_PSWEB.xlsx
+++ b/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/AREAS_PSWEB/20.15.00/accreditamento-checklist_AREAS_PSWEB.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26207"/>
   <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0EF8FF15-A7B8-4616-87F1-66CF11E06E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prerequisiti" sheetId="1" r:id="rId1"/>
@@ -15,7 +16,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TestCases!$A$9:$O$41</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,12 +37,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="E9" authorId="0">
+    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -57,7 +58,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J9" authorId="0">
+    <comment ref="J9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -73,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N9" authorId="0">
+    <comment ref="N9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -99,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="218">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -358,7 +359,16 @@
     </r>
   </si>
   <si>
-    <t>Viene segnalato un errore di connessione al gateway e si chiede all'utente di provare più tardi.</t>
+    <t>2023-02-08T18:14:02Z</t>
+  </si>
+  <si>
+    <t>bcc3f19bba7d21be</t>
+  </si>
+  <si>
+    <t>UNKNOWN_WORKFLOW_ID</t>
+  </si>
+  <si>
+    <t>Viene segnalato un errore di connessione al gateway e si chiede di segnalare il problema all'amministratore di sistema.</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_VPS_KO</t>
@@ -406,6 +416,12 @@
     </r>
   </si>
   <si>
+    <t>2023-02-08T18:18:48Z</t>
+  </si>
+  <si>
+    <t>59076d5918ca5b45</t>
+  </si>
+  <si>
     <t>VALIDAZIONE_VPS_TIMEOUT</t>
   </si>
   <si>
@@ -449,6 +465,9 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.150.4.4.d5b84f6c2c82b17531c09844ba6d7fb8646a32e91125723771c7142eb5c0952d.7fe5c9f725^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Viene mostrato a video l'errore di validazione ottenuto e richiesto all'utente di correggere il dato prima di riprovare</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_VPS_CT7_KO</t>
@@ -905,16 +924,13 @@
   </si>
   <si>
     <t>NO</t>
-  </si>
-  <si>
-    <t>Viene mostrato a video l'errore di validazione ottenuto e richiesto all'utente di correggere il dato prima di riprovare</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -970,6 +986,11 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -1336,7 +1357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -1431,28 +1452,31 @@
     <xf numFmtId="11" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1508,12 +1532,12 @@
     </dxf>
   </dxfs>
   <tableStyles count="2">
-    <tableStyle name="Sheet1-style" pivot="0" count="3">
+    <tableStyle name="Sheet1-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="headerRow" dxfId="5"/>
       <tableStyleElement type="firstRowStripe" dxfId="4"/>
       <tableStyleElement type="secondRowStripe" dxfId="3"/>
     </tableStyle>
-    <tableStyle name="Sheet1-style 2" pivot="0" count="3">
+    <tableStyle name="Sheet1-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
       <tableStyleElement type="headerRow" dxfId="2"/>
       <tableStyleElement type="firstRowStripe" dxfId="1"/>
       <tableStyleElement type="secondRowStripe" dxfId="0"/>
@@ -1531,18 +1555,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A1:A3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:A3">
   <tableColumns count="1">
-    <tableColumn id="1" name="ESITO"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ESITO"/>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_2" displayName="Table_2" ref="B1:B3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_2" displayName="Table_2" ref="B1:B3">
   <tableColumns count="1">
-    <tableColumn id="1" name="APPLICABILITA'"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="APPLICABILITA'"/>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style 2" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1745,7 +1769,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2816,21 +2840,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O886"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="F34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E14" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="46.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
     <col min="4" max="4" width="63.85546875" customWidth="1"/>
     <col min="5" max="5" width="104.7109375" customWidth="1"/>
     <col min="6" max="9" width="33.28515625" customWidth="1"/>
@@ -2857,9 +2881,9 @@
       <c r="A2" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="41"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="44"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -2872,14 +2896,14 @@
       <c r="O2" s="6"/>
     </row>
     <row r="3" spans="1:15" ht="19.5" hidden="1" customHeight="1">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="49" t="s">
+      <c r="B3" s="45"/>
+      <c r="C3" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="41"/>
+      <c r="D3" s="44"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -2892,12 +2916,12 @@
       <c r="O3" s="6"/>
     </row>
     <row r="4" spans="1:15" ht="14.25" hidden="1" customHeight="1">
-      <c r="A4" s="45"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="49" t="s">
+      <c r="A4" s="46"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="41"/>
+      <c r="D4" s="44"/>
       <c r="E4" s="2"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -2911,12 +2935,12 @@
       <c r="O4" s="6"/>
     </row>
     <row r="5" spans="1:15" ht="14.25" hidden="1" customHeight="1">
-      <c r="A5" s="47"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49" t="s">
+      <c r="A5" s="48"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="41"/>
+      <c r="D5" s="44"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -2929,8 +2953,8 @@
       <c r="O5" s="6"/>
     </row>
     <row r="6" spans="1:15" ht="14.25" hidden="1" customHeight="1">
-      <c r="A6" s="38"/>
-      <c r="B6" s="39"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="50"/>
       <c r="C6" s="10"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -3051,12 +3075,10 @@
       </c>
       <c r="L10" s="19"/>
       <c r="M10" s="19"/>
-      <c r="N10" s="20" t="s">
-        <v>35</v>
-      </c>
+      <c r="N10" s="20"/>
       <c r="O10" s="21"/>
     </row>
-    <row r="11" spans="1:15" ht="14.25" customHeight="1">
+    <row r="11" spans="1:15" ht="137.25">
       <c r="A11" s="14">
         <v>25</v>
       </c>
@@ -3090,12 +3112,10 @@
       </c>
       <c r="L11" s="19"/>
       <c r="M11" s="19"/>
-      <c r="N11" s="20" t="s">
-        <v>35</v>
-      </c>
+      <c r="N11" s="20"/>
       <c r="O11" s="21"/>
     </row>
-    <row r="12" spans="1:15" ht="14.25" customHeight="1">
+    <row r="12" spans="1:15" ht="137.25">
       <c r="A12" s="14">
         <v>26</v>
       </c>
@@ -3129,12 +3149,10 @@
       </c>
       <c r="L12" s="19"/>
       <c r="M12" s="19"/>
-      <c r="N12" s="20" t="s">
-        <v>35</v>
-      </c>
+      <c r="N12" s="20"/>
       <c r="O12" s="21"/>
     </row>
-    <row r="13" spans="1:15" ht="14.25" customHeight="1">
+    <row r="13" spans="1:15" ht="137.25">
       <c r="A13" s="14">
         <v>27</v>
       </c>
@@ -3168,12 +3186,10 @@
       </c>
       <c r="L13" s="19"/>
       <c r="M13" s="19"/>
-      <c r="N13" s="20" t="s">
-        <v>35</v>
-      </c>
+      <c r="N13" s="20"/>
       <c r="O13" s="21"/>
     </row>
-    <row r="14" spans="1:15" ht="14.25" customHeight="1">
+    <row r="14" spans="1:15" ht="121.5">
       <c r="A14" s="14">
         <v>35</v>
       </c>
@@ -3189,12 +3205,20 @@
       <c r="E14" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F14" s="17"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
+      <c r="F14" s="17">
+        <v>44965.759745370371</v>
+      </c>
+      <c r="G14" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="I14" s="38" t="s">
+        <v>55</v>
+      </c>
       <c r="J14" s="19" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="K14" s="19" t="s">
         <v>35</v>
@@ -3206,7 +3230,7 @@
       </c>
       <c r="O14" s="21"/>
     </row>
-    <row r="15" spans="1:15" ht="14.25" customHeight="1">
+    <row r="15" spans="1:15" ht="121.5">
       <c r="A15" s="14">
         <v>43</v>
       </c>
@@ -3217,17 +3241,25 @@
         <v>29</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E15" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="17">
+        <v>44965.763055555559</v>
+      </c>
+      <c r="G15" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="H15" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="17"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
       <c r="J15" s="19" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="K15" s="19" t="s">
         <v>35</v>
@@ -3239,7 +3271,7 @@
       </c>
       <c r="O15" s="21"/>
     </row>
-    <row r="16" spans="1:15" ht="14.25" customHeight="1">
+    <row r="16" spans="1:15" ht="45.75">
       <c r="A16" s="14">
         <v>51</v>
       </c>
@@ -3250,17 +3282,17 @@
         <v>29</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="F16" s="17"/>
       <c r="G16" s="18"/>
       <c r="H16" s="18"/>
       <c r="I16" s="18"/>
       <c r="J16" s="19" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="K16" s="19" t="s">
         <v>35</v>
@@ -3272,7 +3304,7 @@
       </c>
       <c r="O16" s="21"/>
     </row>
-    <row r="17" spans="1:15" ht="14.25" customHeight="1">
+    <row r="17" spans="1:15" ht="106.5">
       <c r="A17" s="14">
         <v>122</v>
       </c>
@@ -3283,25 +3315,25 @@
         <v>29</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="F17" s="17">
         <v>44957.650347222225</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I17" s="18" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="J17" s="19" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="K17" s="19" t="s">
         <v>35</v>
@@ -3313,7 +3345,7 @@
       </c>
       <c r="O17" s="21"/>
     </row>
-    <row r="18" spans="1:15" ht="14.25" customHeight="1">
+    <row r="18" spans="1:15" ht="106.5">
       <c r="A18" s="14">
         <v>123</v>
       </c>
@@ -3324,24 +3356,26 @@
         <v>29</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="F18" s="17">
         <v>44957.652974537035</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="I18" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="J18" s="19"/>
+        <v>74</v>
+      </c>
+      <c r="J18" s="19" t="s">
+        <v>75</v>
+      </c>
       <c r="K18" s="19" t="s">
         <v>35</v>
       </c>
@@ -3352,7 +3386,7 @@
       </c>
       <c r="O18" s="21"/>
     </row>
-    <row r="19" spans="1:15" ht="14.25" customHeight="1">
+    <row r="19" spans="1:15" ht="106.5">
       <c r="A19" s="14">
         <v>124</v>
       </c>
@@ -3363,24 +3397,26 @@
         <v>29</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="F19" s="17">
         <v>44958.395162037035</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="H19" s="18" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="I19" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="J19" s="19"/>
+        <v>80</v>
+      </c>
+      <c r="J19" s="19" t="s">
+        <v>75</v>
+      </c>
       <c r="K19" s="19" t="s">
         <v>35</v>
       </c>
@@ -3391,7 +3427,7 @@
       </c>
       <c r="O19" s="21"/>
     </row>
-    <row r="20" spans="1:15" ht="14.25" customHeight="1">
+    <row r="20" spans="1:15" ht="121.5">
       <c r="A20" s="14">
         <v>125</v>
       </c>
@@ -3402,25 +3438,25 @@
         <v>29</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="F20" s="17">
         <v>44958.399363425924</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="I20" s="18" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="J20" s="19" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="K20" s="19" t="s">
         <v>35</v>
@@ -3432,7 +3468,7 @@
       </c>
       <c r="O20" s="21"/>
     </row>
-    <row r="21" spans="1:15" ht="14.25" customHeight="1">
+    <row r="21" spans="1:15" ht="106.5">
       <c r="A21" s="14">
         <v>126</v>
       </c>
@@ -3443,24 +3479,26 @@
         <v>29</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="F21" s="17">
         <v>44957.666134259256</v>
       </c>
       <c r="G21" s="18" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="I21" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="J21" s="19"/>
+        <v>91</v>
+      </c>
+      <c r="J21" s="19" t="s">
+        <v>75</v>
+      </c>
       <c r="K21" s="19" t="s">
         <v>35</v>
       </c>
@@ -3482,25 +3520,25 @@
         <v>29</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F22" s="17">
         <v>44957.671157407407</v>
       </c>
       <c r="G22" s="18" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="I22" s="18" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="J22" s="19" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="K22" s="19" t="s">
         <v>35</v>
@@ -3523,25 +3561,25 @@
         <v>29</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="F23" s="17">
         <v>44957.67628472222</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="J23" s="19" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="K23" s="19" t="s">
         <v>35</v>
@@ -3564,25 +3602,25 @@
         <v>29</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="F24" s="17">
         <v>44957.680532407408</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="H24" s="18" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="J24" s="19" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="K24" s="19" t="s">
         <v>35</v>
@@ -3605,25 +3643,25 @@
         <v>29</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="F25" s="17">
         <v>44957.685115740744</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="H25" s="18" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="I25" s="18" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="J25" s="19" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="K25" s="19" t="s">
         <v>35</v>
@@ -3635,7 +3673,7 @@
       </c>
       <c r="O25" s="21"/>
     </row>
-    <row r="26" spans="1:15" ht="14.25" customHeight="1">
+    <row r="26" spans="1:15" ht="106.5">
       <c r="A26" s="14">
         <v>131</v>
       </c>
@@ -3646,25 +3684,25 @@
         <v>29</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="F26" s="17">
         <v>44957.690057870372</v>
       </c>
       <c r="G26" s="18" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="I26" s="18" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="J26" s="19" t="s">
-        <v>212</v>
+        <v>75</v>
       </c>
       <c r="K26" s="19" t="s">
         <v>35</v>
@@ -3676,7 +3714,7 @@
       </c>
       <c r="O26" s="21"/>
     </row>
-    <row r="27" spans="1:15" ht="14.25" customHeight="1">
+    <row r="27" spans="1:15" ht="106.5">
       <c r="A27" s="14">
         <v>132</v>
       </c>
@@ -3687,25 +3725,25 @@
         <v>29</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="F27" s="17">
         <v>44957.694675925923</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="I27" s="18" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="J27" s="19" t="s">
-        <v>212</v>
+        <v>75</v>
       </c>
       <c r="K27" s="19" t="s">
         <v>35</v>
@@ -3717,7 +3755,7 @@
       </c>
       <c r="O27" s="21"/>
     </row>
-    <row r="28" spans="1:15" ht="14.25" customHeight="1">
+    <row r="28" spans="1:15" ht="121.5">
       <c r="A28" s="14">
         <v>133</v>
       </c>
@@ -3728,25 +3766,25 @@
         <v>29</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="F28" s="17">
         <v>44957.699953703705</v>
       </c>
       <c r="G28" s="18" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="H28" s="18" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="I28" s="18" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="J28" s="19" t="s">
-        <v>212</v>
+        <v>75</v>
       </c>
       <c r="K28" s="19" t="s">
         <v>35</v>
@@ -3758,7 +3796,7 @@
       </c>
       <c r="O28" s="21"/>
     </row>
-    <row r="29" spans="1:15" ht="14.25" customHeight="1">
+    <row r="29" spans="1:15" ht="106.5">
       <c r="A29" s="14">
         <v>134</v>
       </c>
@@ -3769,25 +3807,25 @@
         <v>29</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="F29" s="17">
         <v>44957.70511574074</v>
       </c>
       <c r="G29" s="18" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="I29" s="18" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="J29" s="19" t="s">
-        <v>212</v>
+        <v>75</v>
       </c>
       <c r="K29" s="19" t="s">
         <v>35</v>
@@ -3799,7 +3837,7 @@
       </c>
       <c r="O29" s="21"/>
     </row>
-    <row r="30" spans="1:15" ht="14.25" customHeight="1">
+    <row r="30" spans="1:15" ht="106.5">
       <c r="A30" s="14">
         <v>135</v>
       </c>
@@ -3810,25 +3848,25 @@
         <v>29</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F30" s="17">
         <v>44957.710428240738</v>
       </c>
       <c r="G30" s="18" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="H30" s="18" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="I30" s="18" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="J30" s="19" t="s">
-        <v>212</v>
+        <v>75</v>
       </c>
       <c r="K30" s="19" t="s">
         <v>35</v>
@@ -3840,7 +3878,7 @@
       </c>
       <c r="O30" s="21"/>
     </row>
-    <row r="31" spans="1:15" ht="14.25" customHeight="1">
+    <row r="31" spans="1:15" ht="106.5">
       <c r="A31" s="14">
         <v>136</v>
       </c>
@@ -3851,25 +3889,25 @@
         <v>29</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="F31" s="17">
         <v>44957.715532407405</v>
       </c>
       <c r="G31" s="18" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="H31" s="18" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="I31" s="18" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="J31" s="19" t="s">
-        <v>212</v>
+        <v>75</v>
       </c>
       <c r="K31" s="19" t="s">
         <v>35</v>
@@ -3881,7 +3919,7 @@
       </c>
       <c r="O31" s="21"/>
     </row>
-    <row r="32" spans="1:15" ht="14.25" customHeight="1">
+    <row r="32" spans="1:15" ht="121.5">
       <c r="A32" s="14">
         <v>137</v>
       </c>
@@ -3892,25 +3930,25 @@
         <v>29</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="F32" s="17">
         <v>44958.406157407408</v>
       </c>
       <c r="G32" s="18" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="I32" s="18" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="J32" s="19" t="s">
-        <v>212</v>
+        <v>75</v>
       </c>
       <c r="K32" s="19" t="s">
         <v>35</v>
@@ -3933,25 +3971,25 @@
         <v>29</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="F33" s="17">
         <v>44958.411608796298</v>
       </c>
       <c r="G33" s="18" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="H33" s="18" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="I33" s="18" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="J33" s="19" t="s">
-        <v>212</v>
+        <v>75</v>
       </c>
       <c r="K33" s="19" t="s">
         <v>35</v>
@@ -3974,25 +4012,25 @@
         <v>29</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="F34" s="17">
         <v>44958.416481481479</v>
       </c>
       <c r="G34" s="18" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="H34" s="18" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="I34" s="18" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="J34" s="19" t="s">
-        <v>212</v>
+        <v>75</v>
       </c>
       <c r="K34" s="19" t="s">
         <v>35</v>
@@ -4015,25 +4053,25 @@
         <v>29</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="F35" s="17">
         <v>44958.421168981484</v>
       </c>
       <c r="G35" s="18" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="H35" s="18" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="I35" s="18" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="J35" s="19" t="s">
-        <v>212</v>
+        <v>75</v>
       </c>
       <c r="K35" s="19" t="s">
         <v>35</v>
@@ -4045,7 +4083,7 @@
       </c>
       <c r="O35" s="21"/>
     </row>
-    <row r="36" spans="1:15" ht="14.25" customHeight="1">
+    <row r="36" spans="1:15" ht="121.5">
       <c r="A36" s="14">
         <v>141</v>
       </c>
@@ -4056,25 +4094,25 @@
         <v>29</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="F36" s="17">
         <v>44958.426261574074</v>
       </c>
       <c r="G36" s="18" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="H36" s="18" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="I36" s="18" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="J36" s="19" t="s">
-        <v>212</v>
+        <v>75</v>
       </c>
       <c r="K36" s="19" t="s">
         <v>35</v>
@@ -4086,7 +4124,7 @@
       </c>
       <c r="O36" s="21"/>
     </row>
-    <row r="37" spans="1:15" ht="14.25" customHeight="1">
+    <row r="37" spans="1:15" ht="106.5">
       <c r="A37" s="14">
         <v>142</v>
       </c>
@@ -4097,25 +4135,25 @@
         <v>29</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="F37" s="17">
         <v>44958.430844907409</v>
       </c>
       <c r="G37" s="18" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="H37" s="18" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="I37" s="18" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="J37" s="19" t="s">
-        <v>212</v>
+        <v>75</v>
       </c>
       <c r="K37" s="19" t="s">
         <v>35</v>
@@ -4127,7 +4165,7 @@
       </c>
       <c r="O37" s="21"/>
     </row>
-    <row r="38" spans="1:15" ht="14.25" customHeight="1">
+    <row r="38" spans="1:15" ht="106.5">
       <c r="A38" s="14">
         <v>143</v>
       </c>
@@ -4138,25 +4176,25 @@
         <v>29</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="E38" s="16" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="F38" s="17">
         <v>44958.435497685183</v>
       </c>
       <c r="G38" s="18" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="H38" s="18" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="I38" s="18" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="J38" s="19" t="s">
-        <v>212</v>
+        <v>75</v>
       </c>
       <c r="K38" s="19" t="s">
         <v>35</v>
@@ -4168,7 +4206,7 @@
       </c>
       <c r="O38" s="21"/>
     </row>
-    <row r="39" spans="1:15" ht="14.25" customHeight="1">
+    <row r="39" spans="1:15" ht="106.5">
       <c r="A39" s="14">
         <v>144</v>
       </c>
@@ -4179,25 +4217,25 @@
         <v>29</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="E39" s="16" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="F39" s="17">
         <v>44958.440081018518</v>
       </c>
       <c r="G39" s="18" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="H39" s="18" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="I39" s="18" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="J39" s="19" t="s">
-        <v>212</v>
+        <v>75</v>
       </c>
       <c r="K39" s="19" t="s">
         <v>35</v>
@@ -4209,7 +4247,7 @@
       </c>
       <c r="O39" s="21"/>
     </row>
-    <row r="40" spans="1:15" ht="14.25" customHeight="1">
+    <row r="40" spans="1:15" ht="121.5">
       <c r="A40" s="14">
         <v>145</v>
       </c>
@@ -4220,25 +4258,25 @@
         <v>29</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="F40" s="17">
         <v>44958.445173611108</v>
       </c>
       <c r="G40" s="18" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="H40" s="18" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="I40" s="18" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="J40" s="19" t="s">
-        <v>212</v>
+        <v>75</v>
       </c>
       <c r="K40" s="19" t="s">
         <v>35</v>
@@ -4250,7 +4288,7 @@
       </c>
       <c r="O40" s="21"/>
     </row>
-    <row r="41" spans="1:15" ht="14.25" customHeight="1">
+    <row r="41" spans="1:15" ht="121.5">
       <c r="A41" s="14">
         <v>146</v>
       </c>
@@ -4261,25 +4299,25 @@
         <v>29</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="F41" s="17">
         <v>44958.449374999997</v>
       </c>
       <c r="G41" s="18" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="H41" s="18" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="I41" s="18" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="J41" s="19" t="s">
-        <v>212</v>
+        <v>75</v>
       </c>
       <c r="K41" s="19" t="s">
         <v>35</v>
@@ -14432,7 +14470,7 @@
       <c r="O886" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:O41"/>
+  <autoFilter ref="A9:O41" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="7">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A2:B2"/>
@@ -14449,7 +14487,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14474,80 +14512,80 @@
         <v>14</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1">
       <c r="A2" s="25" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1">
       <c r="A3" s="29" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1">
       <c r="A4" s="29" t="s">
+        <v>204</v>
+      </c>
+      <c r="B4" s="30" t="s">
         <v>198</v>
       </c>
-      <c r="B4" s="30" t="s">
-        <v>192</v>
-      </c>
       <c r="C4" s="31" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1">
       <c r="A5" s="29" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1">
       <c r="A6" s="29" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1">
@@ -14555,13 +14593,13 @@
         <v>29</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.25" customHeight="1"/>
@@ -15562,7 +15600,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -15584,7 +15622,7 @@
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1">
       <c r="A2" s="36" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="B2" s="36" t="s">
         <v>35</v>
@@ -15592,10 +15630,10 @@
     </row>
     <row r="3" spans="1:2" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
chiarimenti casi ID [51 122 123 129]
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/AREAS_PSWEB/20.15.00/accreditamento-checklist_AREAS_PSWEB.xlsx
+++ b/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/AREAS_PSWEB/20.15.00/accreditamento-checklist_AREAS_PSWEB.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lavoro\2022_BTU\FSE2_0 CDA\PSWEB\new FILES\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A62FEAB-9384-4E4F-ABFA-0AE0F9395BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prerequisiti" sheetId="1" r:id="rId1"/>
@@ -16,32 +22,16 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TestCases!$A$9:$O$41</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataSignature="AMtx7mhXj7RfszpgZKzxg8oD/Tet7lb94w=="/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="E9" authorId="0">
+    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -57,7 +47,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J9" authorId="0">
+    <comment ref="J9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -73,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N9" authorId="0">
+    <comment ref="N9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -392,9 +382,6 @@
 Per questo caso di test è richiesta la  sola descrizione del comportamento a fronte di un timeout, da inserire nella colonna "J" nominata come "GESTIONE ERRORE".</t>
   </si>
   <si>
-    <t>Viene segnalato un errore di timeout e si chiede all'utente di provare più tardi.</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_VPS_CT5_KO</t>
   </si>
   <si>
@@ -409,9 +396,6 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.150.4.4.d5b84f6c2c82b17531c09844ba6d7fb8646a32e91125723771c7142eb5c0952d.1d0594e781^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>Viene richiesto all'operatore di valorizzare il campo mancante CF, STP o ENI. Se non abilitato dovrà rivolgersi ad un operatore abilitato alla modifica anagrafica dei pazienti.</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_VPS_CT6_KO</t>
@@ -540,9 +524,6 @@
     <t>2.16.840.1.113883.2.9.2.150.4.4.d5b84f6c2c82b17531c09844ba6d7fb8646a32e91125723771c7142eb5c0952d.43f98cc11f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>Viene segnalato all'operatore un problema sull'assenza del codice fiscale della sua utenza. L'operatore non è autonomo nella risoluzione bensì è necessario un intervento di configurazione.</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_VPS_CT13_KO</t>
   </si>
   <si>
@@ -923,12 +904,21 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.150.4.4.58a5b20a972c56347437f1f3f82187cc925f516c8d8cdd7dd5624de520cb217f.597c2df631^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Viene richiesto all'operatore di corregere il campo CF, STP o ENI. Se non abilitato dovrà rivolgersi ad un operatore abilitato alla modifica anagrafica dei pazienti.</t>
+  </si>
+  <si>
+    <t>Viene segnalato un errore di timeout, ma il flusso applicativo prosegue con la produzione del referto</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Il referto non viene prodotto e un messaggio a video indica  all'utente un problema sull'assenza del codice fiscale della sua utenza. Viene invitato a contattare l'amministratore di sistema e a riprovare dopo la risoluzione</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="11">
     <font>
       <sz val="11"/>
@@ -1356,7 +1346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -1457,24 +1447,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1531,12 +1527,12 @@
     </dxf>
   </dxfs>
   <tableStyles count="2">
-    <tableStyle name="Sheet1-style" pivot="0" count="3">
+    <tableStyle name="Sheet1-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="headerRow" dxfId="5"/>
       <tableStyleElement type="firstRowStripe" dxfId="4"/>
       <tableStyleElement type="secondRowStripe" dxfId="3"/>
     </tableStyle>
-    <tableStyle name="Sheet1-style 2" pivot="0" count="3">
+    <tableStyle name="Sheet1-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
       <tableStyleElement type="headerRow" dxfId="2"/>
       <tableStyleElement type="firstRowStripe" dxfId="1"/>
       <tableStyleElement type="secondRowStripe" dxfId="0"/>
@@ -1554,18 +1550,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A1:A3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:A3">
   <tableColumns count="1">
-    <tableColumn id="1" name="ESITO"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ESITO"/>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_2" displayName="Table_2" ref="B1:B3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_2" displayName="Table_2" ref="B1:B3">
   <tableColumns count="1">
-    <tableColumn id="1" name="APPLICABILITA'"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="APPLICABILITA'"/>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style 2" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1768,7 +1764,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2839,14 +2835,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O886"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2981,7 +2977,7 @@
       <c r="N7" s="9"/>
       <c r="O7" s="6"/>
     </row>
-    <row r="8" spans="1:15" ht="14.25" customHeight="1">
+    <row r="8" spans="1:15" ht="14.25" customHeight="1" thickBot="1">
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
@@ -2993,7 +2989,7 @@
       <c r="N8" s="9"/>
       <c r="O8" s="6"/>
     </row>
-    <row r="9" spans="1:15" ht="14.25" customHeight="1">
+    <row r="9" spans="1:15" ht="14.25" customHeight="1" thickBot="1">
       <c r="A9" s="11" t="s">
         <v>13</v>
       </c>
@@ -3060,13 +3056,13 @@
         <v>44993</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="J10" s="19"/>
       <c r="K10" s="19" t="s">
@@ -3097,13 +3093,13 @@
         <v>44995</v>
       </c>
       <c r="G11" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="H11" s="18" t="s">
         <v>209</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="I11" s="18" t="s">
         <v>212</v>
-      </c>
-      <c r="I11" s="18" t="s">
-        <v>215</v>
       </c>
       <c r="J11" s="19"/>
       <c r="K11" s="19" t="s">
@@ -3134,13 +3130,13 @@
         <v>44995</v>
       </c>
       <c r="G12" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="H12" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="H12" s="37" t="s">
+      <c r="I12" s="18" t="s">
         <v>213</v>
-      </c>
-      <c r="I12" s="18" t="s">
-        <v>216</v>
       </c>
       <c r="J12" s="19"/>
       <c r="K12" s="19" t="s">
@@ -3171,13 +3167,13 @@
         <v>44995</v>
       </c>
       <c r="G13" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="H13" s="18" t="s">
         <v>211</v>
       </c>
-      <c r="H13" s="18" t="s">
+      <c r="I13" s="18" t="s">
         <v>214</v>
-      </c>
-      <c r="I13" s="18" t="s">
-        <v>217</v>
       </c>
       <c r="J13" s="19"/>
       <c r="K13" s="19" t="s">
@@ -3229,7 +3225,7 @@
       </c>
       <c r="O14" s="21"/>
     </row>
-    <row r="15" spans="1:15" ht="135">
+    <row r="15" spans="1:15" ht="135.75" thickBot="1">
       <c r="A15" s="14">
         <v>43</v>
       </c>
@@ -3270,7 +3266,7 @@
       </c>
       <c r="O15" s="21"/>
     </row>
-    <row r="16" spans="1:15" ht="60">
+    <row r="16" spans="1:15" ht="60.75" thickBot="1">
       <c r="A16" s="14">
         <v>51</v>
       </c>
@@ -3290,8 +3286,8 @@
       <c r="G16" s="18"/>
       <c r="H16" s="18"/>
       <c r="I16" s="18"/>
-      <c r="J16" s="19" t="s">
-        <v>51</v>
+      <c r="J16" s="51" t="s">
+        <v>216</v>
       </c>
       <c r="K16" s="19" t="s">
         <v>32</v>
@@ -3303,7 +3299,7 @@
       </c>
       <c r="O16" s="21"/>
     </row>
-    <row r="17" spans="1:15" ht="105">
+    <row r="17" spans="1:15" ht="105.75" thickBot="1">
       <c r="A17" s="14">
         <v>122</v>
       </c>
@@ -3314,25 +3310,25 @@
         <v>29</v>
       </c>
       <c r="D17" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="16" t="s">
         <v>52</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>53</v>
       </c>
       <c r="F17" s="17">
         <v>44957.650347222225</v>
       </c>
       <c r="G17" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="18" t="s">
+      <c r="I17" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="I17" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="J17" s="19" t="s">
-        <v>57</v>
+      <c r="J17" s="51" t="s">
+        <v>61</v>
       </c>
       <c r="K17" s="19" t="s">
         <v>32</v>
@@ -3344,7 +3340,7 @@
       </c>
       <c r="O17" s="21"/>
     </row>
-    <row r="18" spans="1:15" ht="105">
+    <row r="18" spans="1:15" ht="105.75" thickBot="1">
       <c r="A18" s="14">
         <v>123</v>
       </c>
@@ -3355,25 +3351,25 @@
         <v>29</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F18" s="17">
         <v>44957.652974537035</v>
       </c>
       <c r="G18" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="I18" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="H18" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="I18" s="18" t="s">
-        <v>62</v>
-      </c>
       <c r="J18" s="19" t="s">
-        <v>63</v>
+        <v>215</v>
       </c>
       <c r="K18" s="19" t="s">
         <v>32</v>
@@ -3385,7 +3381,7 @@
       </c>
       <c r="O18" s="21"/>
     </row>
-    <row r="19" spans="1:15" ht="105">
+    <row r="19" spans="1:15" ht="105.75" thickBot="1">
       <c r="A19" s="14">
         <v>124</v>
       </c>
@@ -3396,25 +3392,25 @@
         <v>29</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F19" s="17">
         <v>44958.395162037035</v>
       </c>
       <c r="G19" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="H19" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="I19" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="H19" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="I19" s="18" t="s">
-        <v>68</v>
-      </c>
       <c r="J19" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K19" s="19" t="s">
         <v>32</v>
@@ -3437,25 +3433,25 @@
         <v>29</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F20" s="17">
         <v>44958.399363425924</v>
       </c>
       <c r="G20" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="I20" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="H20" s="18" t="s">
+      <c r="J20" s="19" t="s">
         <v>72</v>
-      </c>
-      <c r="I20" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="J20" s="19" t="s">
-        <v>74</v>
       </c>
       <c r="K20" s="19" t="s">
         <v>32</v>
@@ -3478,25 +3474,25 @@
         <v>29</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F21" s="17">
         <v>44957.666134259256</v>
       </c>
       <c r="G21" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="I21" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="H21" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="I21" s="18" t="s">
-        <v>79</v>
-      </c>
       <c r="J21" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K21" s="19" t="s">
         <v>32</v>
@@ -3519,25 +3515,25 @@
         <v>29</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F22" s="17">
         <v>44957.671157407407</v>
       </c>
       <c r="G22" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="I22" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="H22" s="18" t="s">
+      <c r="J22" s="19" t="s">
         <v>83</v>
-      </c>
-      <c r="I22" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="J22" s="19" t="s">
-        <v>85</v>
       </c>
       <c r="K22" s="19" t="s">
         <v>32</v>
@@ -3549,7 +3545,7 @@
       </c>
       <c r="O22" s="21"/>
     </row>
-    <row r="23" spans="1:15" ht="131.25" customHeight="1">
+    <row r="23" spans="1:15" ht="131.25" customHeight="1" thickBot="1">
       <c r="A23" s="14">
         <v>128</v>
       </c>
@@ -3560,25 +3556,25 @@
         <v>29</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F23" s="17">
         <v>44957.67628472222</v>
       </c>
       <c r="G23" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="H23" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="I23" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="H23" s="18" t="s">
+      <c r="J23" s="19" t="s">
         <v>89</v>
-      </c>
-      <c r="I23" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="J23" s="19" t="s">
-        <v>91</v>
       </c>
       <c r="K23" s="19" t="s">
         <v>32</v>
@@ -3590,7 +3586,7 @@
       </c>
       <c r="O23" s="21"/>
     </row>
-    <row r="24" spans="1:15" ht="138" customHeight="1">
+    <row r="24" spans="1:15" ht="138" customHeight="1" thickBot="1">
       <c r="A24" s="14">
         <v>129</v>
       </c>
@@ -3601,25 +3597,25 @@
         <v>29</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F24" s="17">
         <v>44957.680532407408</v>
       </c>
       <c r="G24" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="H24" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="I24" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="H24" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="I24" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="J24" s="19" t="s">
-        <v>97</v>
+      <c r="J24" s="52" t="s">
+        <v>217</v>
       </c>
       <c r="K24" s="19" t="s">
         <v>32</v>
@@ -3631,7 +3627,7 @@
       </c>
       <c r="O24" s="21"/>
     </row>
-    <row r="25" spans="1:15" ht="115.5" customHeight="1">
+    <row r="25" spans="1:15" ht="115.5" customHeight="1" thickBot="1">
       <c r="A25" s="14">
         <v>130</v>
       </c>
@@ -3642,25 +3638,25 @@
         <v>29</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F25" s="17">
         <v>44957.685115740744</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H25" s="18" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I25" s="18" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="J25" s="19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K25" s="19" t="s">
         <v>32</v>
@@ -3672,7 +3668,7 @@
       </c>
       <c r="O25" s="21"/>
     </row>
-    <row r="26" spans="1:15" ht="105">
+    <row r="26" spans="1:15" ht="105.75" thickBot="1">
       <c r="A26" s="14">
         <v>131</v>
       </c>
@@ -3683,25 +3679,25 @@
         <v>29</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F26" s="17">
         <v>44957.690057870372</v>
       </c>
       <c r="G26" s="18" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I26" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J26" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K26" s="19" t="s">
         <v>32</v>
@@ -3724,25 +3720,25 @@
         <v>29</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F27" s="17">
         <v>44957.694675925923</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I27" s="18" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="J27" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K27" s="19" t="s">
         <v>32</v>
@@ -3765,25 +3761,25 @@
         <v>29</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F28" s="17">
         <v>44957.699953703705</v>
       </c>
       <c r="G28" s="18" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H28" s="18" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="I28" s="18" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="J28" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K28" s="19" t="s">
         <v>32</v>
@@ -3806,25 +3802,25 @@
         <v>29</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F29" s="17">
         <v>44957.70511574074</v>
       </c>
       <c r="G29" s="18" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I29" s="18" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="J29" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K29" s="19" t="s">
         <v>32</v>
@@ -3847,25 +3843,25 @@
         <v>29</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F30" s="17">
         <v>44957.710428240738</v>
       </c>
       <c r="G30" s="18" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H30" s="18" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I30" s="18" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="J30" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K30" s="19" t="s">
         <v>32</v>
@@ -3888,25 +3884,25 @@
         <v>29</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F31" s="17">
         <v>44957.715532407405</v>
       </c>
       <c r="G31" s="18" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H31" s="18" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="I31" s="18" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="J31" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K31" s="19" t="s">
         <v>32</v>
@@ -3929,25 +3925,25 @@
         <v>29</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F32" s="17">
         <v>44958.406157407408</v>
       </c>
       <c r="G32" s="18" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I32" s="18" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J32" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K32" s="19" t="s">
         <v>32</v>
@@ -3970,25 +3966,25 @@
         <v>29</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F33" s="17">
         <v>44958.411608796298</v>
       </c>
       <c r="G33" s="18" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="H33" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="I33" s="18" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="J33" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K33" s="19" t="s">
         <v>32</v>
@@ -4011,25 +4007,25 @@
         <v>29</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F34" s="17">
         <v>44958.416481481479</v>
       </c>
       <c r="G34" s="18" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H34" s="18" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="I34" s="18" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="J34" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K34" s="19" t="s">
         <v>32</v>
@@ -4052,25 +4048,25 @@
         <v>29</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F35" s="17">
         <v>44958.421168981484</v>
       </c>
       <c r="G35" s="18" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H35" s="18" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="I35" s="18" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="J35" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K35" s="19" t="s">
         <v>32</v>
@@ -4093,25 +4089,25 @@
         <v>29</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F36" s="17">
         <v>44958.426261574074</v>
       </c>
       <c r="G36" s="18" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H36" s="18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="I36" s="18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J36" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K36" s="19" t="s">
         <v>32</v>
@@ -4134,25 +4130,25 @@
         <v>29</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F37" s="17">
         <v>44958.430844907409</v>
       </c>
       <c r="G37" s="18" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H37" s="18" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I37" s="18" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="J37" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K37" s="19" t="s">
         <v>32</v>
@@ -4175,25 +4171,25 @@
         <v>29</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E38" s="16" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F38" s="17">
         <v>44958.435497685183</v>
       </c>
       <c r="G38" s="18" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H38" s="18" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="I38" s="18" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="J38" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K38" s="19" t="s">
         <v>32</v>
@@ -4216,25 +4212,25 @@
         <v>29</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E39" s="16" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F39" s="17">
         <v>44958.440081018518</v>
       </c>
       <c r="G39" s="18" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H39" s="18" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="I39" s="18" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="J39" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K39" s="19" t="s">
         <v>32</v>
@@ -4257,25 +4253,25 @@
         <v>29</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F40" s="17">
         <v>44958.445173611108</v>
       </c>
       <c r="G40" s="18" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H40" s="18" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="I40" s="18" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="J40" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K40" s="19" t="s">
         <v>32</v>
@@ -4298,25 +4294,25 @@
         <v>29</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F41" s="17">
         <v>44958.449374999997</v>
       </c>
       <c r="G41" s="18" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H41" s="18" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I41" s="18" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="J41" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K41" s="19" t="s">
         <v>32</v>
@@ -14469,7 +14465,7 @@
       <c r="O886" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:O41"/>
+  <autoFilter ref="A9:O41" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="7">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A2:B2"/>
@@ -14486,7 +14482,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14511,80 +14507,80 @@
         <v>14</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1">
       <c r="A2" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="D2" s="28" t="s">
         <v>185</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>186</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="D2" s="28" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1">
       <c r="A3" s="29" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1">
       <c r="A4" s="29" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1">
       <c r="A5" s="29" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1">
       <c r="A6" s="29" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1">
@@ -14592,13 +14588,13 @@
         <v>29</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.25" customHeight="1"/>
@@ -15599,7 +15595,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -15621,7 +15617,7 @@
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1">
       <c r="A2" s="36" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B2" s="36" t="s">
         <v>32</v>
@@ -15629,10 +15625,10 @@
     </row>
     <row r="3" spans="1:2" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25" customHeight="1">

</xml_diff>